<commit_message>
Initial firmware with necessary peripheral drivers
</commit_message>
<xml_diff>
--- a/Documentation/STM32 pinout overview.xlsx
+++ b/Documentation/STM32 pinout overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\JetsonCar-Firmware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2332A6-094B-4B23-9FD5-50142A6B2648}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D692B-5990-4387-8AC1-40CB82D7C14C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -776,45 +776,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="43.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -843,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>61</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="I8" s="2"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -883,7 +883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -906,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>66</v>
       </c>
@@ -929,7 +929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>87</v>
       </c>
@@ -943,7 +943,7 @@
       <c r="I12" s="2"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>77</v>
       </c>
@@ -969,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -995,7 +995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>78</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="I16" s="2"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
@@ -1103,7 +1103,7 @@
       <c r="I19" s="2"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>80</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="I22" s="2"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>1</v>
       </c>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>81</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>82</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>83</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>67</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
@@ -1330,7 +1330,7 @@
       <c r="I29" s="2"/>
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>71</v>
@@ -1357,7 +1357,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>72</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>97</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
         <v>98</v>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>99</v>
       </c>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>76</v>
       </c>
@@ -1478,7 +1478,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" t="s">
         <v>7</v>
@@ -1502,7 +1502,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>8</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>88</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" t="s">
         <v>89</v>
@@ -1560,7 +1560,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>62</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
         <v>63</v>
@@ -1597,7 +1597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>65</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>95</v>
       </c>

</xml_diff>